<commit_message>
Made some PII descriptions less generic.
</commit_message>
<xml_diff>
--- a/NLP/TOMES_Entity_Dictionary.xlsx
+++ b/NLP/TOMES_Entity_Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="20400" windowHeight="10410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20400" windowHeight="10410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="580">
   <si>
     <t>pattern</t>
   </si>
@@ -1497,9 +1497,6 @@
     <t>deductible</t>
   </si>
   <si>
-    <t>A potential reference to a confidential phrase or acronym.</t>
-  </si>
-  <si>
     <t>PII.personal_health_information</t>
   </si>
   <si>
@@ -1719,9 +1716,6 @@
     <t>PII.social_security_number</t>
   </si>
   <si>
-    <t>A potential reference to a health-related phrase or acronym.</t>
-  </si>
-  <si>
     <t>PII.credit_card_number.txt</t>
   </si>
   <si>
@@ -1741,6 +1735,36 @@
   </si>
   <si>
     <t>PII.social_security_number.txt</t>
+  </si>
+  <si>
+    <t>A potential reference to health-related information.</t>
+  </si>
+  <si>
+    <t>An acronym for Electronic Health Record.</t>
+  </si>
+  <si>
+    <t>An acronym for Electronic Medical Record.</t>
+  </si>
+  <si>
+    <t>An acronym for Electronic Protected Health Information.</t>
+  </si>
+  <si>
+    <t>An acronym for Family Medical Leave Act.</t>
+  </si>
+  <si>
+    <t>An acronym for Protection Health Information.</t>
+  </si>
+  <si>
+    <t>A potential reference to sensitive information.</t>
+  </si>
+  <si>
+    <t>An acronym for Business Continuity Planning.</t>
+  </si>
+  <si>
+    <t>An acronym for Continuity Of Operations.</t>
+  </si>
+  <si>
+    <t>An acronym for Non-Disclosure Agreement.</t>
   </si>
 </sst>
 </file>
@@ -2184,7 +2208,8 @@
   <dimension ref="A1:F319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B261" sqref="B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7515,16 +7540,16 @@
         <v>0253</v>
       </c>
       <c r="B254" s="6" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C254" s="23" t="s">
+        <v>549</v>
+      </c>
+      <c r="D254" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E254" s="18" t="s">
         <v>550</v>
-      </c>
-      <c r="D254" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E254" s="18" t="s">
-        <v>551</v>
       </c>
       <c r="F254" s="18" t="s">
         <v>80</v>
@@ -7536,16 +7561,16 @@
         <v>0254</v>
       </c>
       <c r="B255" s="6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C255" s="23" t="s">
+        <v>551</v>
+      </c>
+      <c r="D255" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E255" s="18" t="s">
         <v>552</v>
-      </c>
-      <c r="D255" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E255" s="18" t="s">
-        <v>553</v>
       </c>
       <c r="F255" s="18" t="s">
         <v>80</v>
@@ -7557,16 +7582,16 @@
         <v>0255</v>
       </c>
       <c r="B256" s="6" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C256" s="22" t="s">
+        <v>553</v>
+      </c>
+      <c r="D256" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E256" s="18" t="s">
         <v>554</v>
-      </c>
-      <c r="D256" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E256" s="18" t="s">
-        <v>555</v>
       </c>
       <c r="F256" s="18" t="s">
         <v>80</v>
@@ -7578,10 +7603,10 @@
         <v>0256</v>
       </c>
       <c r="B257" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C257" s="23" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D257" s="25" t="b">
         <v>1</v>
@@ -7599,16 +7624,16 @@
         <v>0257</v>
       </c>
       <c r="B258" s="6" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C258" s="23" t="s">
+        <v>556</v>
+      </c>
+      <c r="D258" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E258" s="18" t="s">
         <v>557</v>
-      </c>
-      <c r="D258" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E258" s="18" t="s">
-        <v>558</v>
       </c>
       <c r="F258" s="18" t="s">
         <v>80</v>
@@ -7620,16 +7645,16 @@
         <v>0258</v>
       </c>
       <c r="B259" s="6" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C259" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="D259" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E259" s="19" t="s">
         <v>559</v>
-      </c>
-      <c r="D259" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E259" s="19" t="s">
-        <v>560</v>
       </c>
       <c r="F259" s="18" t="s">
         <v>80</v>
@@ -7641,10 +7666,10 @@
         <v>0259</v>
       </c>
       <c r="B260" s="6" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C260" s="23" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D260" s="25" t="b">
         <v>1</v>
@@ -7662,16 +7687,16 @@
         <v>0260</v>
       </c>
       <c r="B261" s="6" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C261" s="23" t="s">
+        <v>561</v>
+      </c>
+      <c r="D261" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E261" s="18" t="s">
         <v>562</v>
-      </c>
-      <c r="D261" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E261" s="18" t="s">
-        <v>563</v>
       </c>
       <c r="F261" s="18" t="s">
         <v>80</v>
@@ -7686,13 +7711,13 @@
         <v>489</v>
       </c>
       <c r="C262" s="21" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="D262" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E262" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F262" s="21" t="s">
         <v>80</v>
@@ -7704,16 +7729,16 @@
         <v>0262</v>
       </c>
       <c r="B263" s="21" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C263" s="21" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="D263" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E263" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F263" s="21" t="s">
         <v>80</v>
@@ -7725,16 +7750,16 @@
         <v>0263</v>
       </c>
       <c r="B264" s="21" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C264" s="21" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="D264" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E264" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F264" s="21" t="s">
         <v>80</v>
@@ -7746,16 +7771,16 @@
         <v>0264</v>
       </c>
       <c r="B265" s="21" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C265" s="21" t="s">
-        <v>564</v>
+        <v>572</v>
       </c>
       <c r="D265" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E265" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F265" s="21" t="s">
         <v>80</v>
@@ -7767,16 +7792,16 @@
         <v>0265</v>
       </c>
       <c r="B266" s="21" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C266" s="21" t="s">
-        <v>564</v>
+        <v>573</v>
       </c>
       <c r="D266" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E266" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F266" s="21" t="s">
         <v>80</v>
@@ -7788,16 +7813,16 @@
         <v>0266</v>
       </c>
       <c r="B267" s="21" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C267" s="21" t="s">
-        <v>564</v>
+        <v>573</v>
       </c>
       <c r="D267" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E267" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F267" s="21" t="s">
         <v>80</v>
@@ -7809,16 +7834,16 @@
         <v>0267</v>
       </c>
       <c r="B268" s="21" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C268" s="21" t="s">
-        <v>564</v>
+        <v>574</v>
       </c>
       <c r="D268" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E268" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F268" s="21" t="s">
         <v>80</v>
@@ -7830,16 +7855,16 @@
         <v>0268</v>
       </c>
       <c r="B269" s="21" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C269" s="21" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="D269" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E269" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F269" s="21" t="s">
         <v>80</v>
@@ -7851,16 +7876,16 @@
         <v>0269</v>
       </c>
       <c r="B270" s="21" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C270" s="21" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="D270" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E270" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F270" s="21" t="s">
         <v>80</v>
@@ -7872,16 +7897,16 @@
         <v>0270</v>
       </c>
       <c r="B271" s="21" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C271" s="21" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="D271" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E271" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F271" s="21" t="s">
         <v>80</v>
@@ -7893,16 +7918,16 @@
         <v>0271</v>
       </c>
       <c r="B272" s="21" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C272" s="21" t="s">
-        <v>564</v>
+        <v>575</v>
       </c>
       <c r="D272" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E272" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F272" s="21" t="s">
         <v>80</v>
@@ -7914,16 +7939,16 @@
         <v>0272</v>
       </c>
       <c r="B273" s="21" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C273" s="21" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="D273" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E273" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F273" s="21" t="s">
         <v>80</v>
@@ -7935,16 +7960,16 @@
         <v>0273</v>
       </c>
       <c r="B274" s="21" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C274" s="21" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="D274" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E274" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F274" s="21" t="s">
         <v>80</v>
@@ -7956,16 +7981,16 @@
         <v>0274</v>
       </c>
       <c r="B275" s="21" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C275" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D275" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E275" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F275" s="21" t="s">
         <v>80</v>
@@ -7977,16 +8002,16 @@
         <v>0275</v>
       </c>
       <c r="B276" s="21" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C276" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D276" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E276" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F276" s="21" t="s">
         <v>80</v>
@@ -7998,16 +8023,16 @@
         <v>0276</v>
       </c>
       <c r="B277" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C277" s="21" t="s">
-        <v>490</v>
+        <v>577</v>
       </c>
       <c r="D277" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E277" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F277" s="21" t="s">
         <v>80</v>
@@ -8019,16 +8044,16 @@
         <v>0277</v>
       </c>
       <c r="B278" s="21" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C278" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D278" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E278" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F278" s="21" t="s">
         <v>80</v>
@@ -8040,16 +8065,16 @@
         <v>0278</v>
       </c>
       <c r="B279" s="21" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C279" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D279" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E279" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F279" s="21" t="s">
         <v>80</v>
@@ -8061,16 +8086,16 @@
         <v>0279</v>
       </c>
       <c r="B280" s="21" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C280" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D280" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E280" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F280" s="21" t="s">
         <v>80</v>
@@ -8082,16 +8107,16 @@
         <v>0280</v>
       </c>
       <c r="B281" s="21" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C281" s="21" t="s">
-        <v>490</v>
+        <v>578</v>
       </c>
       <c r="D281" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E281" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F281" s="21" t="s">
         <v>80</v>
@@ -8103,16 +8128,16 @@
         <v>0281</v>
       </c>
       <c r="B282" s="21" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C282" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D282" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E282" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F282" s="21" t="s">
         <v>80</v>
@@ -8124,16 +8149,16 @@
         <v>0282</v>
       </c>
       <c r="B283" s="21" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C283" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D283" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E283" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F283" s="21" t="s">
         <v>80</v>
@@ -8145,16 +8170,16 @@
         <v>0283</v>
       </c>
       <c r="B284" s="21" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C284" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D284" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E284" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F284" s="21" t="s">
         <v>80</v>
@@ -8166,16 +8191,16 @@
         <v>0284</v>
       </c>
       <c r="B285" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C285" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D285" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E285" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F285" s="21" t="s">
         <v>80</v>
@@ -8187,16 +8212,16 @@
         <v>0285</v>
       </c>
       <c r="B286" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C286" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D286" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E286" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F286" s="21" t="s">
         <v>80</v>
@@ -8208,16 +8233,16 @@
         <v>0286</v>
       </c>
       <c r="B287" s="21" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C287" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D287" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E287" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F287" s="21" t="s">
         <v>80</v>
@@ -8229,16 +8254,16 @@
         <v>0287</v>
       </c>
       <c r="B288" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C288" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D288" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E288" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F288" s="21" t="s">
         <v>80</v>
@@ -8250,16 +8275,16 @@
         <v>0288</v>
       </c>
       <c r="B289" s="21" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C289" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D289" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E289" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F289" s="21" t="s">
         <v>80</v>
@@ -8271,16 +8296,16 @@
         <v>0289</v>
       </c>
       <c r="B290" s="21" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C290" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D290" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E290" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F290" s="21" t="s">
         <v>80</v>
@@ -8292,16 +8317,16 @@
         <v>0290</v>
       </c>
       <c r="B291" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C291" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D291" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E291" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F291" s="21" t="s">
         <v>80</v>
@@ -8313,16 +8338,16 @@
         <v>0291</v>
       </c>
       <c r="B292" s="21" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C292" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D292" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E292" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F292" s="21" t="s">
         <v>80</v>
@@ -8334,16 +8359,16 @@
         <v>0292</v>
       </c>
       <c r="B293" s="21" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C293" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D293" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E293" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F293" s="21" t="s">
         <v>80</v>
@@ -8355,16 +8380,16 @@
         <v>0293</v>
       </c>
       <c r="B294" s="21" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C294" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D294" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E294" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F294" s="21" t="s">
         <v>80</v>
@@ -8376,16 +8401,16 @@
         <v>0294</v>
       </c>
       <c r="B295" s="21" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C295" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D295" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E295" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F295" s="21" t="s">
         <v>80</v>
@@ -8397,16 +8422,16 @@
         <v>0295</v>
       </c>
       <c r="B296" s="21" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C296" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D296" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E296" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F296" s="21" t="s">
         <v>80</v>
@@ -8418,16 +8443,16 @@
         <v>0296</v>
       </c>
       <c r="B297" s="21" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C297" s="21" t="s">
-        <v>490</v>
+        <v>579</v>
       </c>
       <c r="D297" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E297" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F297" s="21" t="s">
         <v>80</v>
@@ -8439,16 +8464,16 @@
         <v>0297</v>
       </c>
       <c r="B298" s="21" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C298" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D298" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E298" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F298" s="21" t="s">
         <v>80</v>
@@ -8460,16 +8485,16 @@
         <v>0298</v>
       </c>
       <c r="B299" s="21" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C299" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D299" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E299" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F299" s="21" t="s">
         <v>80</v>
@@ -8481,16 +8506,16 @@
         <v>0299</v>
       </c>
       <c r="B300" s="21" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C300" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D300" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E300" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F300" s="21" t="s">
         <v>80</v>
@@ -8502,16 +8527,16 @@
         <v>0300</v>
       </c>
       <c r="B301" s="21" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C301" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D301" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E301" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F301" s="21" t="s">
         <v>80</v>
@@ -8523,16 +8548,16 @@
         <v>0301</v>
       </c>
       <c r="B302" s="21" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C302" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D302" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E302" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F302" s="21" t="s">
         <v>80</v>
@@ -8544,16 +8569,16 @@
         <v>0302</v>
       </c>
       <c r="B303" s="21" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C303" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D303" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E303" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F303" s="21" t="s">
         <v>80</v>
@@ -8565,16 +8590,16 @@
         <v>0303</v>
       </c>
       <c r="B304" s="21" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C304" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D304" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E304" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F304" s="21" t="s">
         <v>80</v>
@@ -8586,16 +8611,16 @@
         <v>0304</v>
       </c>
       <c r="B305" s="21" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C305" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D305" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E305" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F305" s="21" t="s">
         <v>80</v>
@@ -8607,16 +8632,16 @@
         <v>0305</v>
       </c>
       <c r="B306" s="21" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C306" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D306" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E306" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F306" s="21" t="s">
         <v>80</v>
@@ -8628,16 +8653,16 @@
         <v>0306</v>
       </c>
       <c r="B307" s="21" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C307" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D307" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E307" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F307" s="21" t="s">
         <v>80</v>
@@ -8649,16 +8674,16 @@
         <v>0307</v>
       </c>
       <c r="B308" s="21" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C308" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D308" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E308" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F308" s="21" t="s">
         <v>80</v>
@@ -8670,16 +8695,16 @@
         <v>0308</v>
       </c>
       <c r="B309" s="21" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C309" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D309" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E309" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F309" s="21" t="s">
         <v>80</v>
@@ -8691,16 +8716,16 @@
         <v>0309</v>
       </c>
       <c r="B310" s="21" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C310" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D310" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E310" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F310" s="21" t="s">
         <v>80</v>
@@ -8712,16 +8737,16 @@
         <v>0310</v>
       </c>
       <c r="B311" s="21" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C311" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D311" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E311" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F311" s="21" t="s">
         <v>80</v>
@@ -8733,16 +8758,16 @@
         <v>0311</v>
       </c>
       <c r="B312" s="21" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C312" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D312" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E312" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F312" s="21" t="s">
         <v>80</v>
@@ -8754,16 +8779,16 @@
         <v>0312</v>
       </c>
       <c r="B313" s="21" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C313" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D313" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E313" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F313" s="21" t="s">
         <v>80</v>
@@ -8775,16 +8800,16 @@
         <v>0313</v>
       </c>
       <c r="B314" s="21" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C314" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D314" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E314" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F314" s="21" t="s">
         <v>80</v>
@@ -8796,16 +8821,16 @@
         <v>0314</v>
       </c>
       <c r="B315" s="21" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C315" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D315" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E315" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F315" s="21" t="s">
         <v>80</v>
@@ -8817,16 +8842,16 @@
         <v>0315</v>
       </c>
       <c r="B316" s="21" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C316" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D316" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E316" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F316" s="21" t="s">
         <v>80</v>
@@ -8838,16 +8863,16 @@
         <v>0316</v>
       </c>
       <c r="B317" s="21" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C317" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D317" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E317" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F317" s="21" t="s">
         <v>80</v>
@@ -8859,16 +8884,16 @@
         <v>0317</v>
       </c>
       <c r="B318" s="21" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C318" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D318" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E318" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F318" s="21" t="s">
         <v>80</v>
@@ -8880,16 +8905,16 @@
         <v>0318</v>
       </c>
       <c r="B319" s="21" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C319" s="21" t="s">
-        <v>490</v>
+        <v>576</v>
       </c>
       <c r="D319" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E319" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F319" s="21" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Added regex, modified others.
</commit_message>
<xml_diff>
--- a/NLP/TOMES_Entity_Dictionary.xlsx
+++ b/NLP/TOMES_Entity_Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="20400" windowHeight="10410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="20400" windowHeight="10410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="582">
   <si>
     <t>pattern</t>
   </si>
@@ -1765,6 +1765,12 @@
   </si>
   <si>
     <t>An acronym for Non-Disclosure Agreement.</t>
+  </si>
+  <si>
+    <t>A possible URL string.</t>
+  </si>
+  <si>
+    <t>TOMES.URL</t>
   </si>
 </sst>
 </file>
@@ -2205,11 +2211,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F319"/>
+  <dimension ref="A1:F320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B261" sqref="B261"/>
+      <pane ySplit="1" topLeftCell="A317" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B320" sqref="B320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7620,7 +7626,7 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="6" t="str">
-        <f t="shared" ref="A258:A319" si="4">TEXT(ROW()-1, "0000")</f>
+        <f t="shared" ref="A258:A320" si="4">TEXT(ROW()-1, "0000")</f>
         <v>0257</v>
       </c>
       <c r="B258" s="6" t="s">
@@ -8917,6 +8923,24 @@
         <v>504</v>
       </c>
       <c r="F319" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0319</v>
+      </c>
+      <c r="C320" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="D320" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E320" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="F320" s="6" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>